<commit_message>
final changes for lec 3
</commit_message>
<xml_diff>
--- a/Lecture_Plan.xlsx
+++ b/Lecture_Plan.xlsx
@@ -460,9 +460,6 @@
     <t>LaTex, Markdown, ROxygen</t>
   </si>
   <si>
-    <t>How to use R</t>
-  </si>
-  <si>
     <t>Outline / Plan</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t>Worth mentioning the path control</t>
+  </si>
+  <si>
+    <t>R Fundamentals</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +1873,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,16 +1935,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -2027,7 +2027,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>90</v>
@@ -2042,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>93</v>
@@ -2057,13 +2057,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -2090,10 +2090,10 @@
         <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="F16" s="3"/>
     </row>

</xml_diff>